<commit_message>
started working on marshall1
</commit_message>
<xml_diff>
--- a/apartments.xlsx
+++ b/apartments.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>location</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>provider</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -478,14 +478,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>1.6.33</t>
@@ -498,7 +498,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>107.08</t>
+          <t>107.08 m²</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -516,14 +516,14 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>1.6.32</t>
@@ -536,7 +536,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>38.15</t>
+          <t>38.15 m²</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -554,14 +554,14 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>1.6.31</t>
@@ -574,7 +574,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>39.16</t>
+          <t>39.16 m²</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -592,14 +592,14 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>1.6.30</t>
@@ -612,7 +612,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>36.31</t>
+          <t>36.31 m²</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -630,14 +630,14 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>2.6.36</t>
@@ -650,7 +650,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>36.60</t>
+          <t>36.60 m²</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -668,14 +668,14 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>2.6.37</t>
@@ -688,7 +688,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>91.65</t>
+          <t>91.65 m²</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -706,14 +706,14 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>1.6.29</t>
@@ -726,7 +726,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>91.65</t>
+          <t>91.65 m²</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -744,14 +744,14 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>2.6.35</t>
@@ -764,7 +764,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>43.07</t>
+          <t>43.07 m²</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -782,14 +782,14 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>3.6.24</t>
@@ -802,7 +802,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>123.33</t>
+          <t>123.33 m²</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -820,14 +820,14 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>4.6.18</t>
@@ -840,7 +840,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>101.92</t>
+          <t>101.92 m²</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -858,14 +858,14 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>3.6.21</t>
@@ -878,7 +878,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>69.43</t>
+          <t>69.43 m²</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -896,14 +896,14 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>3.6.22</t>
@@ -916,7 +916,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>59.11</t>
+          <t>59.11 m²</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -934,14 +934,14 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>3.6.23</t>
@@ -954,7 +954,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>54.46</t>
+          <t>54.46 m²</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -972,14 +972,14 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>4.6.17</t>
@@ -992,7 +992,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>90.48</t>
+          <t>90.48 m²</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -1010,14 +1010,14 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>4.6.16</t>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>112.69</t>
+          <t>112.69 m²</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -1048,14 +1048,14 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>5.6.24</t>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>111.79</t>
+          <t>111.79 m²</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -1086,14 +1086,14 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>5.6.22</t>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>55.86</t>
+          <t>55.86 m²</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
@@ -1124,14 +1124,14 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>2.6.32</t>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>65.76</t>
+          <t>65.76 m²</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
@@ -1162,14 +1162,14 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>2.6.33</t>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>64.12</t>
+          <t>64.12 m²</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -1200,14 +1200,14 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>2.6.34</t>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>92.43</t>
+          <t>92.43 m²</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -1238,14 +1238,14 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>5.6.23</t>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>55.51</t>
+          <t>55.51 m²</t>
         </is>
       </c>
       <c r="F22" t="inlineStr"/>
@@ -1276,14 +1276,14 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>5.6.21</t>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>113.43</t>
+          <t>113.43 m²</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1314,14 +1314,14 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>6.6.24</t>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>122.15</t>
+          <t>122.15 m²</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1352,14 +1352,14 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>6.6.23</t>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>86.76</t>
+          <t>86.76 m²</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
@@ -1390,14 +1390,14 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>6.6.22</t>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>68.42</t>
+          <t>68.42 m²</t>
         </is>
       </c>
       <c r="F26" t="inlineStr"/>
@@ -1428,14 +1428,14 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>6.6.21</t>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>96.33</t>
+          <t>96.33 m²</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
@@ -1466,14 +1466,14 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>1.5.28</t>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>120.08</t>
+          <t>120.08 m²</t>
         </is>
       </c>
       <c r="F28" t="inlineStr"/>
@@ -1504,14 +1504,14 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>1.5.27</t>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>38.15</t>
+          <t>38.15 m²</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -1542,14 +1542,14 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>1.5.26</t>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>39.16</t>
+          <t>39.16 m²</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -1580,14 +1580,14 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>1.5.25</t>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>36.31</t>
+          <t>36.31 m²</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -1618,14 +1618,14 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>1.5.24</t>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>100.79</t>
+          <t>100.79 m²</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
@@ -1656,14 +1656,14 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>2.5.30</t>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>36.60</t>
+          <t>36.60 m²</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1694,14 +1694,14 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>2.5.31</t>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>100.79</t>
+          <t>100.79 m²</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -1732,14 +1732,14 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>2.5.29</t>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>43.07</t>
+          <t>43.07 m²</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1770,14 +1770,14 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>3.5.20</t>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>123.33</t>
+          <t>123.33 m²</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
@@ -1808,14 +1808,14 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>4.5.15</t>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>101.92</t>
+          <t>101.92 m²</t>
         </is>
       </c>
       <c r="F37" t="inlineStr"/>
@@ -1846,14 +1846,14 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C38" t="inlineStr">
         <is>
           <t>4.5.14</t>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>90.48</t>
+          <t>90.48 m²</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -1884,14 +1884,14 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>3.5.17</t>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>69.43</t>
+          <t>69.43 m²</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
@@ -1922,14 +1922,14 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>3.5.19</t>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>54.46</t>
+          <t>54.46 m²</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -1960,14 +1960,14 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>3.5.18</t>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>59.11</t>
+          <t>59.11 m²</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -1998,14 +1998,14 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>4.5.13</t>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>112.69</t>
+          <t>112.69 m²</t>
         </is>
       </c>
       <c r="F42" t="inlineStr"/>
@@ -2036,14 +2036,14 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>2.5.26</t>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>65.76</t>
+          <t>65.76 m²</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -2074,14 +2074,14 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C44" t="inlineStr">
         <is>
           <t>2.5.27</t>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>64.12</t>
+          <t>64.12 m²</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -2112,14 +2112,14 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C45" t="inlineStr">
         <is>
           <t>2.5.28</t>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>92.43</t>
+          <t>92.43 m²</t>
         </is>
       </c>
       <c r="F45" t="inlineStr"/>
@@ -2150,14 +2150,14 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>6.5.17</t>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>96.33</t>
+          <t>96.33 m²</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -2188,14 +2188,14 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>5.5.20</t>
@@ -2208,7 +2208,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>111.78</t>
+          <t>111.78 m²</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
@@ -2226,14 +2226,14 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>5.5.19</t>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>55.51</t>
+          <t>55.51 m²</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
@@ -2264,14 +2264,14 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C49" t="inlineStr">
         <is>
           <t>5.5.18</t>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>55.86</t>
+          <t>55.86 m²</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -2302,14 +2302,14 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>5.5.17</t>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>113.43</t>
+          <t>113.43 m²</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -2340,14 +2340,14 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>6.5.20</t>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>121.99</t>
+          <t>121.99 m²</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
@@ -2378,14 +2378,14 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>6.5.18</t>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>68.42</t>
+          <t>68.42 m²</t>
         </is>
       </c>
       <c r="F52" t="inlineStr"/>
@@ -2416,14 +2416,14 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>6.5.19</t>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>86.77</t>
+          <t>86.77 m²</t>
         </is>
       </c>
       <c r="F53" t="inlineStr"/>
@@ -2454,14 +2454,14 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>1.4.23</t>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>125.32</t>
+          <t>125.32 m²</t>
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
@@ -2492,14 +2492,14 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>1.4.22</t>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>38.15</t>
+          <t>38.15 m²</t>
         </is>
       </c>
       <c r="F55" t="inlineStr"/>
@@ -2530,14 +2530,14 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>1.4.21</t>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>39.16</t>
+          <t>39.16 m²</t>
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
@@ -2568,14 +2568,14 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>1.4.20</t>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>36.31</t>
+          <t>36.31 m²</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
@@ -2606,14 +2606,14 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>2.4.23</t>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>36.60</t>
+          <t>36.60 m²</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
@@ -2644,14 +2644,14 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>2.4.22</t>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>43.07</t>
+          <t>43.07 m²</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -2682,14 +2682,14 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>2.4.19</t>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>67.24</t>
+          <t>67.24 m²</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -2720,14 +2720,14 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C61" t="inlineStr">
         <is>
           <t>3.4.16</t>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>123.33</t>
+          <t>123.33 m²</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2758,14 +2758,14 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>3.4.15</t>
@@ -2778,7 +2778,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>54.46</t>
+          <t>54.46 m²</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2796,14 +2796,14 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>3.4.14</t>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>59.11</t>
+          <t>59.11 m²</t>
         </is>
       </c>
       <c r="F63" t="inlineStr"/>
@@ -2834,14 +2834,14 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C64" t="inlineStr">
         <is>
           <t>3.4.13</t>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>69.43</t>
+          <t>69.43 m²</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -2872,14 +2872,14 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>4.4.11</t>
@@ -2892,7 +2892,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>90.48</t>
+          <t>90.48 m²</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
@@ -2910,14 +2910,14 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>4.4.12</t>
@@ -2930,7 +2930,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>101.92</t>
+          <t>101.92 m²</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
@@ -2948,14 +2948,14 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>4.4.10</t>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>112.68</t>
+          <t>112.68 m²</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
@@ -2986,14 +2986,14 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>1.4.19</t>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>64.18</t>
+          <t>64.18 m²</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -3024,14 +3024,14 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>1.4.18</t>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>39.07</t>
+          <t>39.07 m²</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
@@ -3062,14 +3062,14 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>2.4.24</t>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>64.18</t>
+          <t>64.18 m²</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
@@ -3100,14 +3100,14 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>2.4.25</t>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>39.07</t>
+          <t>39.07 m²</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -3138,14 +3138,14 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>2.4.20</t>
@@ -3158,7 +3158,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>64.05</t>
+          <t>64.05 m²</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
@@ -3176,14 +3176,14 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>2.4.21</t>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>92.43</t>
+          <t>92.43 m²</t>
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
@@ -3214,14 +3214,14 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>5.4.16</t>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>111.76</t>
+          <t>111.76 m²</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
@@ -3252,14 +3252,14 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>5.4.15</t>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>55.52</t>
+          <t>55.52 m²</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
@@ -3290,14 +3290,14 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C76" t="inlineStr">
         <is>
           <t>6.4.15</t>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>86.77</t>
+          <t>86.77 m²</t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
@@ -3328,14 +3328,14 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C77" t="inlineStr">
         <is>
           <t>5.4.14</t>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>55.68</t>
+          <t>55.68 m²</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
@@ -3366,14 +3366,14 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>5.4.13</t>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>113.43</t>
+          <t>113.43 m²</t>
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
@@ -3404,14 +3404,14 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>6.4.16</t>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>121.99</t>
+          <t>121.99 m²</t>
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
@@ -3442,14 +3442,14 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>6.4.13</t>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>96.33</t>
+          <t>96.33 m²</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -3480,14 +3480,14 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>6.4.14</t>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>68.42</t>
+          <t>68.42 m²</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
@@ -3518,14 +3518,14 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>2.3.12</t>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>66.45</t>
+          <t>66.45 m²</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
@@ -3556,14 +3556,14 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>2.3.15</t>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>42.85</t>
+          <t>42.85 m²</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
@@ -3594,14 +3594,14 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>2.3.16</t>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>36.59</t>
+          <t>36.59 m²</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
@@ -3632,14 +3632,14 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>1.3.14</t>
@@ -3652,7 +3652,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>36.13</t>
+          <t>36.13 m²</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -3670,14 +3670,14 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>1.3.15</t>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>38.98</t>
+          <t>38.98 m²</t>
         </is>
       </c>
       <c r="F86" t="inlineStr"/>
@@ -3708,14 +3708,14 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C87" t="inlineStr">
         <is>
           <t>1.3.16</t>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>37.97</t>
+          <t>37.97 m²</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -3746,14 +3746,14 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C88" t="inlineStr">
         <is>
           <t>1.3.17</t>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>124.38</t>
+          <t>124.38 m²</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
@@ -3784,14 +3784,14 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>3.3.12</t>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>122.51</t>
+          <t>122.51 m²</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -3822,14 +3822,14 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>3.3.11</t>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>54.17</t>
+          <t>54.17 m²</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
@@ -3860,14 +3860,14 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>3.3.10</t>
@@ -3880,7 +3880,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>58.83</t>
+          <t>58.83 m²</t>
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
@@ -3898,14 +3898,14 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>3.3.09</t>
@@ -3918,7 +3918,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>68.97</t>
+          <t>68.97 m²</t>
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
@@ -3936,14 +3936,14 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>4.3.09</t>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>100.95</t>
+          <t>100.95 m²</t>
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
@@ -3974,14 +3974,14 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>4.3.08</t>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>90.19</t>
+          <t>90.19 m²</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
@@ -4012,14 +4012,14 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C95" t="inlineStr">
         <is>
           <t>4.3.07</t>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>112.01</t>
+          <t>112.01 m²</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -4050,14 +4050,14 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>1.3.13</t>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>63.93</t>
+          <t>63.93 m²</t>
         </is>
       </c>
       <c r="F96" t="inlineStr"/>
@@ -4088,14 +4088,14 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>1.3.12</t>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>38.69</t>
+          <t>38.69 m²</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -4126,14 +4126,14 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C98" t="inlineStr">
         <is>
           <t>2.3.17</t>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>63.92</t>
+          <t>63.92 m²</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -4164,14 +4164,14 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>2.3.18</t>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>38.69</t>
+          <t>38.69 m²</t>
         </is>
       </c>
       <c r="F99" t="inlineStr"/>
@@ -4202,14 +4202,14 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>2.3.13</t>
@@ -4222,7 +4222,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>63.76</t>
+          <t>63.76 m²</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
@@ -4240,14 +4240,14 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C101" t="inlineStr">
         <is>
           <t>2.3.14</t>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>91.83</t>
+          <t>91.83 m²</t>
         </is>
       </c>
       <c r="F101" t="inlineStr"/>
@@ -4278,14 +4278,14 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>5.3.12</t>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>111.07</t>
+          <t>111.07 m²</t>
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
@@ -4316,14 +4316,14 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>5.3.11</t>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>55.23</t>
+          <t>55.23 m²</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
@@ -4354,14 +4354,14 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>5.3.10</t>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>55.57</t>
+          <t>55.57 m²</t>
         </is>
       </c>
       <c r="F104" t="inlineStr"/>
@@ -4392,14 +4392,14 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>6.3.11</t>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>85.70</t>
+          <t>85.70 m²</t>
         </is>
       </c>
       <c r="F105" t="inlineStr"/>
@@ -4430,14 +4430,14 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>6.3.10</t>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>68.12</t>
+          <t>68.12 m²</t>
         </is>
       </c>
       <c r="F106" t="inlineStr"/>
@@ -4468,14 +4468,14 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C107" t="inlineStr">
         <is>
           <t>6.3.09</t>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>95.42</t>
+          <t>95.42 m²</t>
         </is>
       </c>
       <c r="F107" t="inlineStr"/>
@@ -4506,14 +4506,14 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>6.3.12</t>
@@ -4526,7 +4526,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>121.22</t>
+          <t>121.22 m²</t>
         </is>
       </c>
       <c r="F108" t="inlineStr"/>
@@ -4544,14 +4544,14 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C109" t="inlineStr">
         <is>
           <t>5.3.09</t>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>112.71</t>
+          <t>112.71 m²</t>
         </is>
       </c>
       <c r="F109" t="inlineStr"/>
@@ -4582,14 +4582,14 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C110" t="inlineStr">
         <is>
           <t>1.2.09</t>
@@ -4602,7 +4602,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>38.98</t>
+          <t>38.98 m²</t>
         </is>
       </c>
       <c r="F110" t="inlineStr"/>
@@ -4620,14 +4620,14 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C111" t="inlineStr">
         <is>
           <t>1.2.08</t>
@@ -4640,7 +4640,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>36.13</t>
+          <t>36.13 m²</t>
         </is>
       </c>
       <c r="F111" t="inlineStr"/>
@@ -4658,14 +4658,14 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C112" t="inlineStr">
         <is>
           <t>1.2.11</t>
@@ -4678,7 +4678,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>124.38</t>
+          <t>124.38 m²</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
@@ -4696,14 +4696,14 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C113" t="inlineStr">
         <is>
           <t>2.2.09</t>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>36.42</t>
+          <t>36.42 m²</t>
         </is>
       </c>
       <c r="F113" t="inlineStr"/>
@@ -4734,14 +4734,14 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C114" t="inlineStr">
         <is>
           <t>2.2.08</t>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>42.80</t>
+          <t>42.80 m²</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
@@ -4772,14 +4772,14 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C115" t="inlineStr">
         <is>
           <t>1.2.10</t>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>37.97</t>
+          <t>37.97 m²</t>
         </is>
       </c>
       <c r="F115" t="inlineStr"/>
@@ -4810,14 +4810,14 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>2.2.06</t>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>101.41</t>
+          <t>101.41 m²</t>
         </is>
       </c>
       <c r="F116" t="inlineStr"/>
@@ -4848,14 +4848,14 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C117" t="inlineStr">
         <is>
           <t>2.2.07</t>
@@ -4868,7 +4868,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>122.44</t>
+          <t>122.44 m²</t>
         </is>
       </c>
       <c r="F117" t="inlineStr"/>
@@ -4886,14 +4886,14 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C118" t="inlineStr">
         <is>
           <t>3.2.08</t>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>122.51</t>
+          <t>122.51 m²</t>
         </is>
       </c>
       <c r="F118" t="inlineStr"/>
@@ -4924,14 +4924,14 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C119" t="inlineStr">
         <is>
           <t>3.2.07</t>
@@ -4944,7 +4944,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>54.14</t>
+          <t>54.14 m²</t>
         </is>
       </c>
       <c r="F119" t="inlineStr"/>
@@ -4962,14 +4962,14 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C120" t="inlineStr">
         <is>
           <t>3.2.06</t>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>58.83</t>
+          <t>58.83 m²</t>
         </is>
       </c>
       <c r="F120" t="inlineStr"/>
@@ -5000,14 +5000,14 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C121" t="inlineStr">
         <is>
           <t>3.2.05</t>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>68.97</t>
+          <t>68.97 m²</t>
         </is>
       </c>
       <c r="F121" t="inlineStr"/>
@@ -5038,14 +5038,14 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C122" t="inlineStr">
         <is>
           <t>4.2.06</t>
@@ -5058,7 +5058,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>100.95</t>
+          <t>100.95 m²</t>
         </is>
       </c>
       <c r="F122" t="inlineStr"/>
@@ -5076,14 +5076,14 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C123" t="inlineStr">
         <is>
           <t>4.2.05</t>
@@ -5096,7 +5096,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>90.18</t>
+          <t>90.18 m²</t>
         </is>
       </c>
       <c r="F123" t="inlineStr"/>
@@ -5114,14 +5114,14 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C124" t="inlineStr">
         <is>
           <t>4.2.04</t>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>111.99</t>
+          <t>111.99 m²</t>
         </is>
       </c>
       <c r="F124" t="inlineStr"/>
@@ -5152,14 +5152,14 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C125" t="inlineStr">
         <is>
           <t>6.2.05</t>
@@ -5172,7 +5172,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>95.37</t>
+          <t>95.37 m²</t>
         </is>
       </c>
       <c r="F125" t="inlineStr"/>
@@ -5190,14 +5190,14 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C126" t="inlineStr">
         <is>
           <t>5.2.08</t>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>110.99</t>
+          <t>110.99 m²</t>
         </is>
       </c>
       <c r="F126" t="inlineStr"/>
@@ -5228,14 +5228,14 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>1.2.07</t>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>63.92</t>
+          <t>63.92 m²</t>
         </is>
       </c>
       <c r="F127" t="inlineStr"/>
@@ -5266,14 +5266,14 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C128" t="inlineStr">
         <is>
           <t>2.2.10</t>
@@ -5286,7 +5286,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>63.92</t>
+          <t>63.92 m²</t>
         </is>
       </c>
       <c r="F128" t="inlineStr"/>
@@ -5304,14 +5304,14 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C129" t="inlineStr">
         <is>
           <t>1.2.06</t>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>38.69</t>
+          <t>38.69 m²</t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
@@ -5342,14 +5342,14 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C130" t="inlineStr">
         <is>
           <t>2.2.11</t>
@@ -5362,7 +5362,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>38.69</t>
+          <t>38.69 m²</t>
         </is>
       </c>
       <c r="F130" t="inlineStr"/>
@@ -5380,14 +5380,14 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C131" t="inlineStr">
         <is>
           <t>5.2.07</t>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>55.23</t>
+          <t>55.23 m²</t>
         </is>
       </c>
       <c r="F131" t="inlineStr"/>
@@ -5418,14 +5418,14 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C132" t="inlineStr">
         <is>
           <t>5.2.06</t>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>55.57</t>
+          <t>55.57 m²</t>
         </is>
       </c>
       <c r="F132" t="inlineStr"/>
@@ -5456,14 +5456,14 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C133" t="inlineStr">
         <is>
           <t>6.2.06</t>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>68.12</t>
+          <t>68.12 m²</t>
         </is>
       </c>
       <c r="F133" t="inlineStr"/>
@@ -5494,14 +5494,14 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C134" t="inlineStr">
         <is>
           <t>6.2.07</t>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>85.63</t>
+          <t>85.63 m²</t>
         </is>
       </c>
       <c r="F134" t="inlineStr"/>
@@ -5532,14 +5532,14 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C135" t="inlineStr">
         <is>
           <t>6.2.08</t>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>121.22</t>
+          <t>121.22 m²</t>
         </is>
       </c>
       <c r="F135" t="inlineStr"/>
@@ -5570,14 +5570,14 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C136" t="inlineStr">
         <is>
           <t>5.2.05</t>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>112.67</t>
+          <t>112.67 m²</t>
         </is>
       </c>
       <c r="F136" t="inlineStr"/>
@@ -5608,14 +5608,14 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C137" t="inlineStr">
         <is>
           <t>1.1.04</t>
@@ -5628,7 +5628,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>38.35</t>
+          <t>38.35 m²</t>
         </is>
       </c>
       <c r="F137" t="inlineStr"/>
@@ -5646,14 +5646,14 @@
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C138" t="inlineStr">
         <is>
           <t>1.1.03</t>
@@ -5666,7 +5666,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>39.15</t>
+          <t>39.15 m²</t>
         </is>
       </c>
       <c r="F138" t="inlineStr"/>
@@ -5684,14 +5684,14 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C139" t="inlineStr">
         <is>
           <t>1.1.02</t>
@@ -5704,7 +5704,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>36.59</t>
+          <t>36.59 m²</t>
         </is>
       </c>
       <c r="F139" t="inlineStr"/>
@@ -5722,14 +5722,14 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C140" t="inlineStr">
         <is>
           <t>1.1.05</t>
@@ -5742,7 +5742,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>104.58</t>
+          <t>104.58 m²</t>
         </is>
       </c>
       <c r="F140" t="inlineStr"/>
@@ -5760,14 +5760,14 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
           <t>H1</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>1.1.01</t>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>101.90</t>
+          <t>101.90 m²</t>
         </is>
       </c>
       <c r="F141" t="inlineStr"/>
@@ -5798,14 +5798,14 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C142" t="inlineStr">
         <is>
           <t>2.1.05</t>
@@ -5818,7 +5818,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>102.06</t>
+          <t>102.06 m²</t>
         </is>
       </c>
       <c r="F142" t="inlineStr"/>
@@ -5836,14 +5836,14 @@
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C143" t="inlineStr">
         <is>
           <t>2.1.04</t>
@@ -5856,7 +5856,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>36.59</t>
+          <t>36.59 m²</t>
         </is>
       </c>
       <c r="F143" t="inlineStr"/>
@@ -5874,14 +5874,14 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C144" t="inlineStr">
         <is>
           <t>2.1.03</t>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>45.68</t>
+          <t>45.68 m²</t>
         </is>
       </c>
       <c r="F144" t="inlineStr"/>
@@ -5912,14 +5912,14 @@
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C145" t="inlineStr">
         <is>
           <t>2.1.01</t>
@@ -5932,7 +5932,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>100.75</t>
+          <t>100.75 m²</t>
         </is>
       </c>
       <c r="F145" t="inlineStr"/>
@@ -5950,14 +5950,14 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
           <t>H2</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C146" t="inlineStr">
         <is>
           <t>2.1.02</t>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>113.01</t>
+          <t>113.01 m²</t>
         </is>
       </c>
       <c r="F146" t="inlineStr"/>
@@ -5988,14 +5988,14 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C147" t="inlineStr">
         <is>
           <t>3.1.04</t>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>121.71</t>
+          <t>121.71 m²</t>
         </is>
       </c>
       <c r="F147" t="inlineStr"/>
@@ -6026,14 +6026,14 @@
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C148" t="inlineStr">
         <is>
           <t>3.1.03</t>
@@ -6046,7 +6046,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>41.95</t>
+          <t>41.95 m²</t>
         </is>
       </c>
       <c r="F148" t="inlineStr"/>
@@ -6064,14 +6064,14 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C149" t="inlineStr">
         <is>
           <t>3.1.02</t>
@@ -6084,7 +6084,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>59.70</t>
+          <t>59.70 m²</t>
         </is>
       </c>
       <c r="F149" t="inlineStr"/>
@@ -6102,14 +6102,14 @@
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
           <t>H3</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C150" t="inlineStr">
         <is>
           <t>3.1.01</t>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>66.66</t>
+          <t>66.66 m²</t>
         </is>
       </c>
       <c r="F150" t="inlineStr"/>
@@ -6140,14 +6140,14 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C151" t="inlineStr">
         <is>
           <t>4.1.02</t>
@@ -6160,7 +6160,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>71.94</t>
+          <t>71.94 m²</t>
         </is>
       </c>
       <c r="F151" t="inlineStr"/>
@@ -6178,14 +6178,14 @@
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C152" t="inlineStr">
         <is>
           <t>4.1.03</t>
@@ -6198,7 +6198,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>101.02</t>
+          <t>101.02 m²</t>
         </is>
       </c>
       <c r="F152" t="inlineStr"/>
@@ -6216,14 +6216,14 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
           <t>H4</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C153" t="inlineStr">
         <is>
           <t>4.1.01</t>
@@ -6236,7 +6236,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>110.14</t>
+          <t>110.14 m²</t>
         </is>
       </c>
       <c r="F153" t="inlineStr"/>
@@ -6254,14 +6254,14 @@
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C154" t="inlineStr">
         <is>
           <t>5.1.04</t>
@@ -6274,7 +6274,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>108.83</t>
+          <t>108.83 m²</t>
         </is>
       </c>
       <c r="F154" t="inlineStr"/>
@@ -6292,14 +6292,14 @@
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C155" t="inlineStr">
         <is>
           <t>5.1.03</t>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>56.32</t>
+          <t>56.32 m²</t>
         </is>
       </c>
       <c r="F155" t="inlineStr"/>
@@ -6330,14 +6330,14 @@
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C156" t="inlineStr">
         <is>
           <t>5.1.02</t>
@@ -6350,7 +6350,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>42.98</t>
+          <t>42.98 m²</t>
         </is>
       </c>
       <c r="F156" t="inlineStr"/>
@@ -6368,14 +6368,14 @@
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
           <t>H5</t>
         </is>
       </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C157" t="inlineStr">
         <is>
           <t>5.1.01</t>
@@ -6388,7 +6388,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>113.94</t>
+          <t>113.94 m²</t>
         </is>
       </c>
       <c r="F157" t="inlineStr"/>
@@ -6406,14 +6406,14 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C158" t="inlineStr">
         <is>
           <t>6.1.04</t>
@@ -6426,7 +6426,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>119.50</t>
+          <t>119.50 m²</t>
         </is>
       </c>
       <c r="F158" t="inlineStr"/>
@@ -6444,14 +6444,14 @@
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C159" t="inlineStr">
         <is>
           <t>6.1.01</t>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>95.65</t>
+          <t>95.65 m²</t>
         </is>
       </c>
       <c r="F159" t="inlineStr"/>
@@ -6482,14 +6482,14 @@
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C160" t="inlineStr">
         <is>
           <t>6.1.02</t>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>65.93</t>
+          <t>65.93 m²</t>
         </is>
       </c>
       <c r="F160" t="inlineStr"/>
@@ -6520,14 +6520,14 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
+          <t>franz</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
           <t>H6</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>franz</t>
-        </is>
-      </c>
       <c r="C161" t="inlineStr">
         <is>
           <t>6.1.03</t>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>81.19</t>
+          <t>81.19 m²</t>
         </is>
       </c>
       <c r="F161" t="inlineStr"/>

</xml_diff>